<commit_message>
Added LSI, edited ART
</commit_message>
<xml_diff>
--- a/data_raw/item_banks/ART_itembank.xlsx
+++ b/data_raw/item_banks/ART_itembank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\item_banks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC454EB-D341-4E0E-9025-0226A12E5E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834C7A29-175B-416F-BC0E-D9026B60C427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,19 +16,26 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$1:$C$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$1:$C$66</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="70">
   <si>
     <t>Albert Camus</t>
   </si>
@@ -150,9 +157,6 @@
     <t>Marc Elsberg</t>
   </si>
   <si>
-    <t>Marcus Maurer</t>
-  </si>
-  <si>
     <t>Mark Deuze</t>
   </si>
   <si>
@@ -186,9 +190,6 @@
     <t>Philippe J. Maarek</t>
   </si>
   <si>
-    <t>Rainer Maria Rilke</t>
-  </si>
-  <si>
     <t>Sabina Mihelj</t>
   </si>
   <si>
@@ -204,9 +205,6 @@
     <t>Sigrid Weigel</t>
   </si>
   <si>
-    <t>Stefan Jarolimek</t>
-  </si>
-  <si>
     <t>Stieg Larsson</t>
   </si>
   <si>
@@ -231,124 +229,19 @@
     <t>John R. R. Tolkien</t>
   </si>
   <si>
-    <t>Michael Saitow</t>
-  </si>
-  <si>
     <t>John W. Downey</t>
   </si>
   <si>
-    <t>August Graf von Platen</t>
-  </si>
-  <si>
-    <t>Emanuel Geibel</t>
-  </si>
-  <si>
-    <t>Ernst Moritz Arndt</t>
-  </si>
-  <si>
-    <t>Ernst von Feuchtersleben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friedrich Hebbel </t>
-  </si>
-  <si>
-    <t>Friedrich Rückert</t>
-  </si>
-  <si>
-    <t>Gertrud Kolmar</t>
-  </si>
-  <si>
-    <t>Hans-Eckardt Wenzel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heinrich Heine </t>
-  </si>
-  <si>
-    <t>Hermann Conradi</t>
-  </si>
-  <si>
-    <t>Johanna Ambrosius</t>
-  </si>
-  <si>
-    <t>Johannes R. Becher</t>
-  </si>
-  <si>
-    <t>Joseph von Eichendorff</t>
-  </si>
-  <si>
-    <t>Justinius Kerner</t>
-  </si>
-  <si>
-    <t>Klaus Johann Groth</t>
-  </si>
-  <si>
-    <t>Ludwig Achim von Arnim</t>
-  </si>
-  <si>
-    <t>Ludwig Uhland</t>
-  </si>
-  <si>
-    <t>Luise Hensel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul Celan </t>
-  </si>
-  <si>
-    <t>Wilhelm Hertz</t>
-  </si>
-  <si>
-    <t>poet</t>
-  </si>
-  <si>
-    <t>Stella M. Hurtley</t>
-  </si>
-  <si>
-    <t>Julia Fahrenkamp-Uppenbrink</t>
-  </si>
-  <si>
-    <t>Takuzo Aida</t>
-  </si>
-  <si>
-    <t>Leslie C. Aiello</t>
-  </si>
-  <si>
-    <t>Ray H. Baughman</t>
-  </si>
-  <si>
-    <t>Christian Büchel</t>
-  </si>
-  <si>
-    <t>György Buzsáki</t>
-  </si>
-  <si>
-    <t>James J. Collins</t>
-  </si>
-  <si>
-    <t>Frans de Waal</t>
-  </si>
-  <si>
-    <t>Ernst Ulrich von Weizsäcker</t>
-  </si>
-  <si>
     <t>item_id</t>
   </si>
   <si>
     <t>role</t>
   </si>
   <si>
-    <t>Wilhelm Busch</t>
-  </si>
-  <si>
     <t>foil</t>
   </si>
   <si>
     <t>Michael Sülflow</t>
-  </si>
-  <si>
-    <t>Christian von Ehrenfels</t>
-  </si>
-  <si>
-    <t>Gottfried Philipp von Bülow</t>
   </si>
   <si>
     <t>writer</t>
@@ -678,13 +571,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A104" sqref="A104:XFD108"/>
+      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,13 +590,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,34 +604,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A45" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -747,10 +640,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,10 +652,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -771,10 +664,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,10 +676,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -795,10 +688,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,10 +700,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -819,10 +712,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -831,10 +724,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -843,10 +736,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -855,10 +748,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -867,10 +760,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,10 +772,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -891,10 +784,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -903,10 +796,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -915,10 +808,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -927,10 +820,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,10 +832,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -951,10 +844,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -963,10 +856,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -975,10 +868,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,10 +880,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -999,10 +892,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,10 +904,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1023,10 +916,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1035,10 +928,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1047,10 +940,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1059,10 +952,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1071,10 +964,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,10 +976,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1095,10 +988,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1107,10 +1000,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,10 +1012,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1131,10 +1024,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1143,10 +1036,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,10 +1048,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,10 +1060,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1179,10 +1072,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1191,10 +1084,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1203,10 +1096,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1215,10 +1108,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1227,712 +1120,267 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A46:A66" si="1">A45+1</f>
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C57" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C60" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C62" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C63" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="C64" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C66" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <f t="shared" ref="A68:A103" si="1">A67+1</f>
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="B72" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="B73" t="s">
-        <v>68</v>
-      </c>
-      <c r="C73" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="B74" t="s">
-        <v>36</v>
-      </c>
-      <c r="C74" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="B75" t="s">
-        <v>38</v>
-      </c>
-      <c r="C75" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>41</v>
-      </c>
-      <c r="C76" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="B77" t="s">
-        <v>43</v>
-      </c>
-      <c r="C77" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>104</v>
-      </c>
-      <c r="C78" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="B79" t="s">
-        <v>45</v>
-      </c>
-      <c r="C79" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="B80" t="s">
-        <v>48</v>
-      </c>
-      <c r="C80" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="B81" t="s">
-        <v>49</v>
-      </c>
-      <c r="C81" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="B82" t="s">
-        <v>50</v>
-      </c>
-      <c r="C82" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="B83" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="B84" t="s">
-        <v>53</v>
-      </c>
-      <c r="C84" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="B85" t="s">
-        <v>54</v>
-      </c>
-      <c r="C85" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="B86" t="s">
-        <v>57</v>
-      </c>
-      <c r="C86" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="B87" t="s">
-        <v>58</v>
-      </c>
-      <c r="C87" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="B88" t="s">
-        <v>60</v>
-      </c>
-      <c r="C88" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="B89" t="s">
-        <v>62</v>
-      </c>
-      <c r="C89" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="B90" t="s">
-        <v>95</v>
-      </c>
-      <c r="C90" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="B91" t="s">
-        <v>105</v>
-      </c>
-      <c r="C91" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="B92" t="s">
-        <v>99</v>
-      </c>
-      <c r="C92" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="B93" t="s">
-        <v>98</v>
-      </c>
-      <c r="C93" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="B94" t="s">
-        <v>106</v>
-      </c>
-      <c r="C94" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="B95" t="s">
-        <v>96</v>
-      </c>
-      <c r="C95" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="B96" t="s">
-        <v>97</v>
-      </c>
-      <c r="C96" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="B97" t="s">
-        <v>91</v>
-      </c>
-      <c r="C97" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="B98" t="s">
-        <v>93</v>
-      </c>
-      <c r="C98" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="B99" t="s">
-        <v>40</v>
-      </c>
-      <c r="C99" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="B100" t="s">
-        <v>67</v>
-      </c>
-      <c r="C100" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="B101" t="s">
-        <v>94</v>
-      </c>
-      <c r="C101" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="B102" t="s">
-        <v>90</v>
-      </c>
-      <c r="C102" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="B103" t="s">
-        <v>92</v>
-      </c>
-      <c r="C103" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C103">
-    <sortCondition ref="C2:C103"/>
-    <sortCondition ref="B2:B103"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C66">
+    <sortCondition ref="C2:C66"/>
+    <sortCondition ref="B2:B66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>